<commit_message>
Update jmdc annual health checkup mapping
</commit_message>
<xml_diff>
--- a/docs/JMDC/Vocab Updates/Annual_Health_Checkup_Mapping.xlsx
+++ b/docs/JMDC/Vocab Updates/Annual_Health_Checkup_Mapping.xlsx
@@ -1,29 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10209"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repo_22\GitHub\OHDSI\ETL-LambdaBuilder\docs\JMDC\Vocab Updates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eburrow3/Documents/Git/ETL-LambdaBuilder/docs/JMDC/Vocab Updates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12E88614-F1B2-4400-8E41-18311CEB8DAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0925D838-AAC3-A449-9F2C-46991FB42C67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="856" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-220" yWindow="760" windowWidth="30660" windowHeight="17180" tabRatio="856" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Annual health checkup" sheetId="40" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Annual health checkup'!$A$1:$D$53</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Annual health checkup'!$A$1:$D$57</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="179">
   <si>
     <t>HbA1c</t>
   </si>
@@ -154,36 +154,6 @@
     <phoneticPr fontId="8"/>
   </si>
   <si>
-    <t>Do you habitually smoke? 
-*You habitually smoke if you have ever smoked over 100 cigarettes in total or for six months or more and have also smoked in the last month.</t>
-    <phoneticPr fontId="14"/>
-  </si>
-  <si>
-    <t>Do you have dinner within two hours before going to bed at least three times a week?</t>
-    <phoneticPr fontId="8"/>
-  </si>
-  <si>
-    <t>Do you have a snack (late evening snack other than breakfast, lunch and dinner) after dinner at least three times a week?</t>
-    <phoneticPr fontId="8"/>
-  </si>
-  <si>
-    <t>Do you skip breakfast at least three times a week?</t>
-    <phoneticPr fontId="8"/>
-  </si>
-  <si>
-    <t>How often do you drink (sake, distilled spirit, beer, liqueur)?</t>
-    <phoneticPr fontId="14"/>
-  </si>
-  <si>
-    <t>Amount of drinking per day on days when you drink.
-*1 go of sake is equivalent to: a medium bottle of beer (around 500 mL), 35 degrees of distilled spirit (80 mL), a glass of double whiskey (60 mL), two glasses of wine (240 mL)</t>
-    <phoneticPr fontId="8"/>
-  </si>
-  <si>
-    <t>Speed of eating compared with others</t>
-    <phoneticPr fontId="14"/>
-  </si>
-  <si>
     <t>Getting enough sleep</t>
     <phoneticPr fontId="14"/>
   </si>
@@ -309,12 +279,6 @@
     <phoneticPr fontId="8"/>
   </si>
   <si>
-    <t>1=Every day
-2=Sometimes
-3=Rarely</t>
-    <phoneticPr fontId="8"/>
-  </si>
-  <si>
     <t>Whether there are any medical history.</t>
     <phoneticPr fontId="8"/>
   </si>
@@ -332,13 +296,6 @@
   </si>
   <si>
     <t>Presence_of_objective_symptoms</t>
-    <phoneticPr fontId="8"/>
-  </si>
-  <si>
-    <t>1=Less than 1 go
-2=1 go to less than 2 go
-3=2 go to less than 3 go
-4=3 go or more</t>
     <phoneticPr fontId="8"/>
   </si>
   <si>
@@ -587,38 +544,12 @@
     <t>Fundus_examination(Keith-Wagener_classification)</t>
   </si>
   <si>
-    <t>Smoking_habit</t>
-  </si>
-  <si>
     <t>1=4298794
 2=4222303</t>
   </si>
   <si>
     <t>1=Smoker
 2=Non-smoker</t>
-  </si>
-  <si>
-    <t>Eating1(fast_eating,etc.)</t>
-  </si>
-  <si>
-    <t>1=Fast
-2=Normal
-3=Slow</t>
-  </si>
-  <si>
-    <t>Eating2(before_going_to_bed)</t>
-  </si>
-  <si>
-    <t>Eating3(late_evening_snack/snack)</t>
-  </si>
-  <si>
-    <t>Eating_habit</t>
-  </si>
-  <si>
-    <t>Drinking_habit</t>
-  </si>
-  <si>
-    <t>Amount_of_drinking</t>
   </si>
   <si>
     <t>Sleep</t>
@@ -645,6 +576,169 @@
     <t>1 = 45880745
 2 = 45877108
 3 = 45884578</t>
+  </si>
+  <si>
+    <t>Do you habitually smoke? 
+(Until March 2024)
+(null : Unknown)
+* "Current habitual smokers" are those who have smoked a total of 100 cigarettes or more, or for at least 6 months, and who have smoked for the last month.</t>
+  </si>
+  <si>
+    <t>1 = Yes
+2 = No</t>
+  </si>
+  <si>
+    <t>Do you currently smoke regularly?
+(Since April 2024)
+(null : Unknown) 
+* "Current habitual smokers" are those who meet both conditions 1 and 2.
+Condition 1 : Smoking for the last 1 month.
+Condition 2 : Smoking for more than 6 months in your lifetime, or I smoke more than 100 cigarettes in total.</t>
+  </si>
+  <si>
+    <t>1 = Yes (Condition 1 and Condition 2 are set to Satisfy both)
+2 = I used to smoke, but I haven't smoked for the last 1 month (only condition 2 is satisfied)
+3 = No (other than (1) and (2) )</t>
+  </si>
+  <si>
+    <t>smoking_habit_until_mar_24</t>
+  </si>
+  <si>
+    <t>smoking_habit_after_apr_24</t>
+  </si>
+  <si>
+    <t>1=4298794
+2=4310250
+3=4222303</t>
+  </si>
+  <si>
+    <t>1=Smoker
+2 = Ex-smoker
+3=Non-smoker</t>
+  </si>
+  <si>
+    <t>Yes, Used to smoke, No</t>
+  </si>
+  <si>
+    <t>eating1_fast_eating</t>
+  </si>
+  <si>
+    <t>Speed of eating compared with others.
+(null : Unknown)</t>
+  </si>
+  <si>
+    <t>1 = Fast
+2 = Average
+3 = Slow</t>
+  </si>
+  <si>
+    <t>eating2_before_bedtime</t>
+  </si>
+  <si>
+    <t>Do you have dinner within two hours before going to bed at least three times a week?
+(null : Unknown)</t>
+  </si>
+  <si>
+    <t>eating3_late_evening_snack</t>
+  </si>
+  <si>
+    <t>Do you have a snack (late evening snack other than breakfast, lunch and dinner) after dinner at least three times a week?
+(before 201803) 
+(null : Unknown)</t>
+  </si>
+  <si>
+    <t>eating3_snack</t>
+  </si>
+  <si>
+    <t>Do you have a snack (sweets) or sugary beverages other than breakfast, lunch and dinner?
+(after 201804)
+(null : Unknown)</t>
+  </si>
+  <si>
+    <t>1 = Every day
+2 = Sometimes
+3 = Rarely</t>
+  </si>
+  <si>
+    <t>eating_habit_breakfast</t>
+  </si>
+  <si>
+    <t>Do you skip breakfast at least three times a week?
+(null : Unknown)</t>
+  </si>
+  <si>
+    <t>Every day, Sometimes, Rarely</t>
+  </si>
+  <si>
+    <t>Fast, Average, Slow</t>
+  </si>
+  <si>
+    <t>4288153, 765707 , 763696</t>
+  </si>
+  <si>
+    <t>drinking_habit_until_mar_24</t>
+  </si>
+  <si>
+    <t>How often do you drink (sake, distilled spirit, beer, liqueur) ?
+(Until March 2024)
+(null : Unknown)</t>
+  </si>
+  <si>
+    <t>amount_of_drinking_until_mar_24</t>
+  </si>
+  <si>
+    <t>The amount of alcohol consumed per day on a drinking day.
+(Until March 2024)
+(null : Unknown)</t>
+  </si>
+  <si>
+    <t>1 = Less than 1 go
+2 = 1 go to less than 2 go
+3 = 2 go to less than 3 go
+4 = 3 go or more</t>
+    <phoneticPr fontId="13"/>
+  </si>
+  <si>
+    <t>drinking_habit_after_apr_24</t>
+    <phoneticPr fontId="13"/>
+  </si>
+  <si>
+    <t>Frequently drinking alcohol (Japan sake, shochu, beer, Western sake, etc.) Degree.
+(Since April 2024)
+(null : Unknown)
+* "Quit" refers to those who have not consumed alcoholic beverages for more than one year in the past and who have not consumed alcoholic beverages for more than one year in the past.</t>
+  </si>
+  <si>
+    <t>1 = Daily
+2 = 5~6 days a week
+3 = 3~4 days a week
+4 = 1~2 days a week
+5 = 1~3 days per month
+6 = Less than 1 day per month
+7 = Quit
+8 = Don't drink (can't drink)</t>
+    <phoneticPr fontId="13"/>
+  </si>
+  <si>
+    <t>amount_of_drinking_after_apr_24</t>
+  </si>
+  <si>
+    <t>The amount of alcohol consumed per day on a drinking day.
+(Since April 2024)
+(null : Unknown)</t>
+  </si>
+  <si>
+    <t>1 = 1 is not in the balance
+2 = 1~2 is not in the balance
+3 = 2~3 is not in the balance
+4 = 3~5
+5 = 5 or more</t>
+  </si>
+  <si>
+    <t>Daily, Quit, Don't drink</t>
+  </si>
+  <si>
+    <t>4288153, 4220362 , 4022664</t>
   </si>
 </sst>
 </file>
@@ -654,7 +748,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_(&quot;¥&quot;* #,##0_);_(&quot;¥&quot;* \(#,##0\);_(&quot;¥&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="18">
+  <fonts count="19">
     <font>
       <sz val="11"/>
       <name val="ＭＳ Ｐゴシック"/>
@@ -781,6 +875,12 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <name val="Meiryo UI"/>
+      <family val="3"/>
+      <charset val="128"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -939,7 +1039,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -976,6 +1076,9 @@
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="34">
@@ -1322,32 +1425,32 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:K54"/>
+  <dimension ref="A1:K58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I36" sqref="I36"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12"/>
   <cols>
     <col min="1" max="1" width="25.5" style="2" customWidth="1"/>
     <col min="2" max="2" width="39.5" style="2" customWidth="1"/>
-    <col min="3" max="3" width="15.125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="8.125" style="3" customWidth="1"/>
-    <col min="5" max="5" width="19.875" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="34.875" style="2" customWidth="1"/>
-    <col min="7" max="7" width="16.75" style="2" customWidth="1"/>
+    <col min="3" max="3" width="25.6640625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="8.1640625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="19.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="34.83203125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="16.6640625" style="2" customWidth="1"/>
     <col min="8" max="8" width="38.5" style="2" customWidth="1"/>
-    <col min="9" max="9" width="24.125" style="2" customWidth="1"/>
-    <col min="10" max="10" width="16.625" style="2" customWidth="1"/>
-    <col min="11" max="11" width="4.125" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.125" style="2" customWidth="1"/>
-    <col min="13" max="13" width="32.875" style="2" customWidth="1"/>
+    <col min="9" max="9" width="24.1640625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="16.6640625" style="2" customWidth="1"/>
+    <col min="11" max="11" width="4.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.1640625" style="2" customWidth="1"/>
+    <col min="13" max="13" width="32.83203125" style="2" customWidth="1"/>
     <col min="14" max="14" width="16.5" style="2" customWidth="1"/>
     <col min="15" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1">
+    <row r="1" spans="1:10" s="1" customFormat="1" ht="13">
       <c r="A1" s="4" t="s">
         <v>5</v>
       </c>
@@ -1361,25 +1464,25 @@
         <v>28</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="13">
       <c r="A2" s="6" t="s">
         <v>4</v>
       </c>
@@ -1400,17 +1503,17 @@
         <v>9531</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="I2" s="6"/>
       <c r="J2" s="6"/>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" ht="13">
       <c r="A3" s="6" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="C3" s="6"/>
       <c r="D3" s="7" t="s">
@@ -1420,26 +1523,26 @@
         <v>3016258</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="G3" s="6">
         <v>8582</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="I3" s="6"/>
       <c r="J3" s="6"/>
     </row>
-    <row r="4" spans="1:10" ht="24">
+    <row r="4" spans="1:10" ht="26">
       <c r="A4" s="6" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>29</v>
@@ -1451,15 +1554,15 @@
       <c r="I4" s="6"/>
       <c r="J4" s="6"/>
     </row>
-    <row r="5" spans="1:10" ht="24">
+    <row r="5" spans="1:10" ht="26">
       <c r="A5" s="8" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="D5" s="7" t="s">
         <v>29</v>
@@ -1471,15 +1574,15 @@
       <c r="I5" s="6"/>
       <c r="J5" s="6"/>
     </row>
-    <row r="6" spans="1:10" ht="24">
+    <row r="6" spans="1:10" ht="26">
       <c r="A6" s="8" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="D6" s="7" t="s">
         <v>29</v>
@@ -1491,7 +1594,7 @@
       <c r="I6" s="6"/>
       <c r="J6" s="6"/>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" ht="13">
       <c r="A7" s="6" t="s">
         <v>12</v>
       </c>
@@ -1506,18 +1609,18 @@
         <v>3004249</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="G7" s="6">
         <v>8876</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="I7" s="6"/>
       <c r="J7" s="6"/>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" ht="13">
       <c r="A8" s="6" t="s">
         <v>13</v>
       </c>
@@ -1532,26 +1635,26 @@
         <v>3012888</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="G8" s="6">
         <v>8876</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="I8" s="6"/>
       <c r="J8" s="6"/>
     </row>
-    <row r="9" spans="1:10" ht="48">
+    <row r="9" spans="1:10" ht="52">
       <c r="A9" s="6" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="D9" s="7" t="s">
         <v>29</v>
@@ -1563,9 +1666,9 @@
       <c r="I9" s="6"/>
       <c r="J9" s="6"/>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" ht="13">
       <c r="A10" s="6" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>1</v>
@@ -1578,18 +1681,18 @@
         <v>3022038</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="G10" s="6">
         <v>8840</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="I10" s="6"/>
       <c r="J10" s="6"/>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" ht="13">
       <c r="A11" s="6" t="s">
         <v>14</v>
       </c>
@@ -1604,18 +1707,18 @@
         <v>3007070</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="G11" s="6">
         <v>8840</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="I11" s="6"/>
       <c r="J11" s="6"/>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" ht="13">
       <c r="A12" s="6" t="s">
         <v>15</v>
       </c>
@@ -1630,23 +1733,23 @@
         <v>3028437</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="G12" s="6">
         <v>8840</v>
       </c>
       <c r="H12" s="6" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="I12" s="6"/>
       <c r="J12" s="6"/>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" ht="13">
       <c r="A13" s="6" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="C13" s="6"/>
       <c r="D13" s="7" t="s">
@@ -1656,23 +1759,23 @@
         <v>3003792</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="G13" s="6">
         <v>8645</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="I13" s="6"/>
       <c r="J13" s="6"/>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" ht="13">
       <c r="A14" s="6" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="C14" s="6"/>
       <c r="D14" s="7" t="s">
@@ -1682,23 +1785,23 @@
         <v>3006923</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="G14" s="6">
         <v>8645</v>
       </c>
       <c r="H14" s="6" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="I14" s="6"/>
       <c r="J14" s="6"/>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" ht="13">
       <c r="A15" s="6" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="C15" s="6"/>
       <c r="D15" s="7" t="s">
@@ -1708,18 +1811,18 @@
         <v>3026910</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="G15" s="6">
         <v>8645</v>
       </c>
       <c r="H15" s="6" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="I15" s="6"/>
       <c r="J15" s="6"/>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" ht="13">
       <c r="A16" s="6" t="s">
         <v>16</v>
       </c>
@@ -1734,18 +1837,18 @@
         <v>3037187</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="G16" s="6">
         <v>8840</v>
       </c>
       <c r="H16" s="6" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="I16" s="6"/>
       <c r="J16" s="6"/>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:10" ht="13">
       <c r="A17" s="6" t="s">
         <v>17</v>
       </c>
@@ -1760,23 +1863,23 @@
         <v>3000483</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="G17" s="6">
         <v>8840</v>
       </c>
       <c r="H17" s="6" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="I17" s="6"/>
       <c r="J17" s="6"/>
     </row>
-    <row r="18" spans="1:10">
+    <row r="18" spans="1:10" ht="13">
       <c r="A18" s="6" t="s">
         <v>0</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="C18" s="6"/>
       <c r="D18" s="7" t="s">
@@ -1792,17 +1895,17 @@
         <v>8554</v>
       </c>
       <c r="H18" s="6" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="I18" s="6"/>
       <c r="J18" s="6"/>
     </row>
-    <row r="19" spans="1:10" ht="60">
+    <row r="19" spans="1:10" ht="65">
       <c r="A19" s="6" t="s">
         <v>18</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="C19" s="6" t="s">
         <v>26</v>
@@ -1814,23 +1917,23 @@
         <v>3020650</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="G19" s="6"/>
       <c r="H19" s="6"/>
       <c r="I19" s="6" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="J19" s="6" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" ht="60">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="65">
       <c r="A20" s="6" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="C20" s="6" t="s">
         <v>26</v>
@@ -1842,23 +1945,23 @@
         <v>3037185</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="G20" s="6"/>
       <c r="H20" s="6"/>
       <c r="I20" s="6" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="J20" s="6" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="13">
       <c r="A21" s="6" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="C21" s="6"/>
       <c r="D21" s="7" t="s">
@@ -1868,23 +1971,23 @@
         <v>3009542</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="G21" s="6">
         <v>8554</v>
       </c>
       <c r="H21" s="6" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="I21" s="6"/>
       <c r="J21" s="6"/>
     </row>
-    <row r="22" spans="1:10">
+    <row r="22" spans="1:10" ht="13">
       <c r="A22" s="6" t="s">
         <v>19</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="C22" s="6"/>
       <c r="D22" s="7" t="s">
@@ -1894,23 +1997,23 @@
         <v>3000963</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="G22" s="6">
         <v>8713</v>
       </c>
       <c r="H22" s="6" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="I22" s="6"/>
       <c r="J22" s="6"/>
     </row>
-    <row r="23" spans="1:10">
+    <row r="23" spans="1:10" ht="13">
       <c r="A23" s="6" t="s">
         <v>20</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="C23" s="6"/>
       <c r="D23" s="7" t="s">
@@ -1920,47 +2023,47 @@
         <v>3026361</v>
       </c>
       <c r="F23" s="6" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="G23" s="6">
         <v>32706</v>
       </c>
       <c r="H23" s="6" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="I23" s="6"/>
       <c r="J23" s="6"/>
     </row>
-    <row r="24" spans="1:10" ht="24">
+    <row r="24" spans="1:10" ht="26">
       <c r="A24" s="6" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="D24" s="7" t="s">
         <v>29</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="F24" s="6" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="G24" s="6"/>
       <c r="H24" s="6"/>
       <c r="I24" s="6"/>
       <c r="J24" s="6"/>
     </row>
-    <row r="25" spans="1:10" ht="72">
+    <row r="25" spans="1:10" ht="78">
       <c r="A25" s="6" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="C25" s="6" t="s">
         <v>25</v>
@@ -1975,12 +2078,12 @@
       <c r="I25" s="6"/>
       <c r="J25" s="6"/>
     </row>
-    <row r="26" spans="1:10" ht="60">
+    <row r="26" spans="1:10" ht="65">
       <c r="A26" s="6" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="C26" s="6" t="s">
         <v>24</v>
@@ -1995,12 +2098,12 @@
       <c r="I26" s="6"/>
       <c r="J26" s="6"/>
     </row>
-    <row r="27" spans="1:10" ht="60">
+    <row r="27" spans="1:10" ht="65">
       <c r="A27" s="6" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="C27" s="6" t="s">
         <v>24</v>
@@ -2015,15 +2118,15 @@
       <c r="I27" s="6"/>
       <c r="J27" s="6"/>
     </row>
-    <row r="28" spans="1:10" ht="108">
+    <row r="28" spans="1:10" ht="117">
       <c r="A28" s="6" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="D28" s="7" t="s">
         <v>29</v>
@@ -2035,192 +2138,212 @@
       <c r="I28" s="6"/>
       <c r="J28" s="6"/>
     </row>
-    <row r="29" spans="1:10" ht="48">
-      <c r="A29" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="B29" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="C29" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="D29" s="7" t="s">
-        <v>29</v>
+    <row r="29" spans="1:10" ht="105">
+      <c r="A29" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="B29" s="13" t="s">
+        <v>142</v>
+      </c>
+      <c r="C29" s="13" t="s">
+        <v>143</v>
+      </c>
+      <c r="D29" s="13" t="s">
+        <v>100</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="F29" s="6" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="G29" s="6"/>
       <c r="H29" s="6"/>
       <c r="I29" s="6"/>
       <c r="J29" s="6" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" ht="36">
-      <c r="A30" s="6" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" ht="180">
+      <c r="A30" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="B30" s="13" t="s">
         <v>144</v>
       </c>
-      <c r="B30" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="C30" s="6" t="s">
+      <c r="C30" s="13" t="s">
         <v>145</v>
       </c>
-      <c r="D30" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="E30" s="6"/>
-      <c r="F30" s="6"/>
+      <c r="D30" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="F30" s="6" t="s">
+        <v>149</v>
+      </c>
       <c r="G30" s="6"/>
       <c r="H30" s="6"/>
       <c r="I30" s="6"/>
-      <c r="J30" s="6"/>
-    </row>
-    <row r="31" spans="1:10" ht="24">
-      <c r="A31" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="B31" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="C31" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="D31" s="7" t="s">
-        <v>29</v>
+      <c r="J30" s="6" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" ht="45">
+      <c r="A31" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="B31" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="C31" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="D31" s="13" t="s">
+        <v>100</v>
       </c>
       <c r="E31" s="6"/>
       <c r="F31" s="6"/>
       <c r="G31" s="6"/>
       <c r="H31" s="6"/>
       <c r="I31" s="6"/>
-      <c r="J31" s="6"/>
-    </row>
-    <row r="32" spans="1:10" ht="36">
-      <c r="A32" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="B32" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C32" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="D32" s="7" t="s">
-        <v>29</v>
+      <c r="J31" s="6" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" ht="45">
+      <c r="A32" s="13" t="s">
+        <v>154</v>
+      </c>
+      <c r="B32" s="13" t="s">
+        <v>155</v>
+      </c>
+      <c r="C32" s="13" t="s">
+        <v>143</v>
+      </c>
+      <c r="D32" s="13" t="s">
+        <v>100</v>
       </c>
       <c r="E32" s="6"/>
       <c r="F32" s="6"/>
       <c r="G32" s="6"/>
       <c r="H32" s="6"/>
-      <c r="I32" s="6"/>
-      <c r="J32" s="6"/>
-    </row>
-    <row r="33" spans="1:10" ht="24">
-      <c r="A33" s="6" t="s">
-        <v>148</v>
-      </c>
-      <c r="B33" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="C33" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="D33" s="7" t="s">
-        <v>29</v>
+      <c r="I32" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="J32" s="6" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" ht="75">
+      <c r="A33" s="13" t="s">
+        <v>156</v>
+      </c>
+      <c r="B33" s="13" t="s">
+        <v>157</v>
+      </c>
+      <c r="C33" s="13" t="s">
+        <v>143</v>
+      </c>
+      <c r="D33" s="13" t="s">
+        <v>100</v>
       </c>
       <c r="E33" s="6"/>
       <c r="F33" s="6"/>
       <c r="G33" s="6"/>
       <c r="H33" s="6"/>
-      <c r="I33" s="6"/>
-      <c r="J33" s="6"/>
-    </row>
-    <row r="34" spans="1:10" ht="36">
-      <c r="A34" s="6" t="s">
-        <v>149</v>
-      </c>
-      <c r="B34" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="C34" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="D34" s="7" t="s">
-        <v>29</v>
+      <c r="I33" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="J33" s="6" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" ht="60">
+      <c r="A34" s="13" t="s">
+        <v>158</v>
+      </c>
+      <c r="B34" s="13" t="s">
+        <v>159</v>
+      </c>
+      <c r="C34" s="13" t="s">
+        <v>160</v>
+      </c>
+      <c r="D34" s="13" t="s">
+        <v>100</v>
       </c>
       <c r="E34" s="6"/>
       <c r="F34" s="6"/>
       <c r="G34" s="6"/>
       <c r="H34" s="6"/>
-      <c r="I34" s="6"/>
-      <c r="J34" s="6"/>
-    </row>
-    <row r="35" spans="1:10" ht="72">
-      <c r="A35" s="6" t="s">
-        <v>150</v>
-      </c>
-      <c r="B35" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="C35" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="D35" s="7" t="s">
-        <v>29</v>
+      <c r="I34" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="J34" s="6" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" ht="30">
+      <c r="A35" s="13" t="s">
+        <v>161</v>
+      </c>
+      <c r="B35" s="13" t="s">
+        <v>162</v>
+      </c>
+      <c r="C35" s="13" t="s">
+        <v>143</v>
+      </c>
+      <c r="D35" s="13" t="s">
+        <v>100</v>
       </c>
       <c r="E35" s="6"/>
       <c r="F35" s="6"/>
       <c r="G35" s="6"/>
       <c r="H35" s="6"/>
-      <c r="I35" s="6"/>
-      <c r="J35" s="6"/>
-    </row>
-    <row r="36" spans="1:10" ht="36">
-      <c r="A36" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="B36" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="C36" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="D36" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="E36" s="6">
-        <v>40764749</v>
-      </c>
-      <c r="F36" s="6" t="s">
+      <c r="I35" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="J35" s="6" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" ht="60">
+      <c r="A36" s="13" t="s">
+        <v>166</v>
+      </c>
+      <c r="B36" s="13" t="s">
+        <v>167</v>
+      </c>
+      <c r="C36" s="13" t="s">
+        <v>160</v>
+      </c>
+      <c r="D36" s="13" t="s">
         <v>100</v>
       </c>
+      <c r="E36" s="6"/>
+      <c r="F36" s="6"/>
       <c r="G36" s="6"/>
       <c r="H36" s="6"/>
       <c r="I36" s="6" t="s">
-        <v>98</v>
+        <v>165</v>
       </c>
       <c r="J36" s="6" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" ht="24">
-      <c r="A37" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="B37" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="C37" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="D37" s="7" t="s">
-        <v>29</v>
+        <v>163</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" ht="90">
+      <c r="A37" s="13" t="s">
+        <v>168</v>
+      </c>
+      <c r="B37" s="13" t="s">
+        <v>169</v>
+      </c>
+      <c r="C37" s="13" t="s">
+        <v>170</v>
+      </c>
+      <c r="D37" s="13" t="s">
+        <v>100</v>
       </c>
       <c r="E37" s="6"/>
       <c r="F37" s="6"/>
@@ -2229,38 +2352,42 @@
       <c r="I37" s="6"/>
       <c r="J37" s="6"/>
     </row>
-    <row r="38" spans="1:10" ht="24">
-      <c r="A38" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="B38" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="C38" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="D38" s="7" t="s">
-        <v>29</v>
+    <row r="38" spans="1:10" ht="120">
+      <c r="A38" s="13" t="s">
+        <v>171</v>
+      </c>
+      <c r="B38" s="13" t="s">
+        <v>172</v>
+      </c>
+      <c r="C38" s="13" t="s">
+        <v>173</v>
+      </c>
+      <c r="D38" s="13" t="s">
+        <v>100</v>
       </c>
       <c r="E38" s="6"/>
       <c r="F38" s="6"/>
       <c r="G38" s="6"/>
       <c r="H38" s="6"/>
-      <c r="I38" s="6"/>
-      <c r="J38" s="6"/>
-    </row>
-    <row r="39" spans="1:10" ht="24">
-      <c r="A39" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="B39" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="C39" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="D39" s="7" t="s">
-        <v>29</v>
+      <c r="I38" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="J38" s="6" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" ht="120">
+      <c r="A39" s="13" t="s">
+        <v>174</v>
+      </c>
+      <c r="B39" s="13" t="s">
+        <v>175</v>
+      </c>
+      <c r="C39" s="13" t="s">
+        <v>176</v>
+      </c>
+      <c r="D39" s="13" t="s">
+        <v>100</v>
       </c>
       <c r="E39" s="6"/>
       <c r="F39" s="6"/>
@@ -2269,35 +2396,43 @@
       <c r="I39" s="6"/>
       <c r="J39" s="6"/>
     </row>
-    <row r="40" spans="1:10" ht="60">
+    <row r="40" spans="1:10" ht="39">
       <c r="A40" s="6" t="s">
-        <v>82</v>
+        <v>134</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="D40" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="E40" s="6"/>
-      <c r="F40" s="6"/>
+      <c r="E40" s="6">
+        <v>40764749</v>
+      </c>
+      <c r="F40" s="6" t="s">
+        <v>91</v>
+      </c>
       <c r="G40" s="6"/>
       <c r="H40" s="6"/>
-      <c r="I40" s="6"/>
-      <c r="J40" s="6"/>
-    </row>
-    <row r="41" spans="1:10" ht="48">
+      <c r="I40" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="J40" s="6" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" ht="26">
       <c r="A41" s="6" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="D41" s="7" t="s">
         <v>29</v>
@@ -2309,15 +2444,15 @@
       <c r="I41" s="6"/>
       <c r="J41" s="6"/>
     </row>
-    <row r="42" spans="1:10" ht="48">
+    <row r="42" spans="1:10" ht="26">
       <c r="A42" s="6" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="D42" s="7" t="s">
         <v>29</v>
@@ -2329,15 +2464,15 @@
       <c r="I42" s="6"/>
       <c r="J42" s="6"/>
     </row>
-    <row r="43" spans="1:10" ht="36">
+    <row r="43" spans="1:10" ht="26">
       <c r="A43" s="6" t="s">
-        <v>11</v>
+        <v>72</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="D43" s="7" t="s">
         <v>29</v>
@@ -2349,15 +2484,15 @@
       <c r="I43" s="6"/>
       <c r="J43" s="6"/>
     </row>
-    <row r="44" spans="1:10" ht="36">
+    <row r="44" spans="1:10" ht="52">
       <c r="A44" s="6" t="s">
-        <v>10</v>
+        <v>73</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="D44" s="7" t="s">
         <v>29</v>
@@ -2369,15 +2504,15 @@
       <c r="I44" s="6"/>
       <c r="J44" s="6"/>
     </row>
-    <row r="45" spans="1:10" ht="48">
+    <row r="45" spans="1:10" ht="52">
       <c r="A45" s="6" t="s">
-        <v>9</v>
+        <v>74</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="D45" s="7" t="s">
         <v>29</v>
@@ -2389,15 +2524,15 @@
       <c r="I45" s="6"/>
       <c r="J45" s="6"/>
     </row>
-    <row r="46" spans="1:10" ht="36">
+    <row r="46" spans="1:10" ht="52">
       <c r="A46" s="6" t="s">
-        <v>8</v>
+        <v>75</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="C46" s="6" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="D46" s="7" t="s">
         <v>29</v>
@@ -2409,15 +2544,15 @@
       <c r="I46" s="6"/>
       <c r="J46" s="6"/>
     </row>
-    <row r="47" spans="1:10" ht="36">
+    <row r="47" spans="1:10" ht="39">
       <c r="A47" s="6" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="C47" s="6" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="D47" s="7" t="s">
         <v>29</v>
@@ -2429,15 +2564,15 @@
       <c r="I47" s="6"/>
       <c r="J47" s="6"/>
     </row>
-    <row r="48" spans="1:10" ht="24">
+    <row r="48" spans="1:10" ht="39">
       <c r="A48" s="6" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="C48" s="6" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="D48" s="7" t="s">
         <v>29</v>
@@ -2449,15 +2584,15 @@
       <c r="I48" s="6"/>
       <c r="J48" s="6"/>
     </row>
-    <row r="49" spans="1:11" ht="96">
+    <row r="49" spans="1:11" ht="39">
       <c r="A49" s="6" t="s">
-        <v>152</v>
+        <v>9</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="C49" s="6" t="s">
-        <v>72</v>
+        <v>53</v>
       </c>
       <c r="D49" s="7" t="s">
         <v>29</v>
@@ -2469,15 +2604,15 @@
       <c r="I49" s="6"/>
       <c r="J49" s="6"/>
     </row>
-    <row r="50" spans="1:11" ht="36">
+    <row r="50" spans="1:11" ht="39">
       <c r="A50" s="6" t="s">
-        <v>153</v>
+        <v>8</v>
       </c>
       <c r="B50" s="6" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="C50" s="6" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="D50" s="7" t="s">
         <v>29</v>
@@ -2489,111 +2624,191 @@
       <c r="I50" s="6"/>
       <c r="J50" s="6"/>
     </row>
-    <row r="51" spans="1:11">
+    <row r="51" spans="1:11" ht="26">
       <c r="A51" s="6" t="s">
-        <v>154</v>
+        <v>7</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="C51" s="6"/>
+        <v>41</v>
+      </c>
+      <c r="C51" s="6" t="s">
+        <v>53</v>
+      </c>
       <c r="D51" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="E51" s="6">
-        <v>3037556</v>
-      </c>
-      <c r="F51" s="6" t="s">
-        <v>155</v>
-      </c>
-      <c r="G51" s="6">
-        <v>8840</v>
-      </c>
-      <c r="H51" s="6" t="s">
-        <v>92</v>
-      </c>
+      <c r="E51" s="6"/>
+      <c r="F51" s="6"/>
+      <c r="G51" s="6"/>
+      <c r="H51" s="6"/>
       <c r="I51" s="6"/>
       <c r="J51" s="6"/>
     </row>
-    <row r="52" spans="1:11">
+    <row r="52" spans="1:11" ht="26">
       <c r="A52" s="6" t="s">
-        <v>156</v>
+        <v>6</v>
       </c>
       <c r="B52" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="C52" s="6"/>
+        <v>42</v>
+      </c>
+      <c r="C52" s="6" t="s">
+        <v>53</v>
+      </c>
       <c r="D52" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="E52" s="6">
-        <v>3016723</v>
-      </c>
-      <c r="F52" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="G52" s="6">
-        <v>8840</v>
-      </c>
-      <c r="H52" s="6" t="s">
-        <v>92</v>
-      </c>
+      <c r="E52" s="6"/>
+      <c r="F52" s="6"/>
+      <c r="G52" s="6"/>
+      <c r="H52" s="6"/>
       <c r="I52" s="6"/>
       <c r="J52" s="6"/>
     </row>
-    <row r="53" spans="1:11">
+    <row r="53" spans="1:11" ht="91">
       <c r="A53" s="6" t="s">
-        <v>21</v>
+        <v>135</v>
       </c>
       <c r="B53" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C53" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="C53" s="6"/>
       <c r="D53" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="E53" s="9">
-        <v>3027114</v>
-      </c>
-      <c r="F53" s="6" t="s">
-        <v>157</v>
-      </c>
-      <c r="G53" s="6">
-        <v>8840</v>
-      </c>
-      <c r="H53" s="6" t="s">
-        <v>92</v>
-      </c>
+      <c r="E53" s="6"/>
+      <c r="F53" s="6"/>
+      <c r="G53" s="6"/>
+      <c r="H53" s="6"/>
       <c r="I53" s="6"/>
       <c r="J53" s="6"/>
-      <c r="K53" s="6"/>
-    </row>
-    <row r="54" spans="1:11" ht="75.95" customHeight="1">
-      <c r="A54" s="10" t="s">
-        <v>107</v>
-      </c>
-      <c r="B54" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="C54" s="10" t="s">
-        <v>108</v>
-      </c>
-      <c r="D54" s="11" t="s">
-        <v>109</v>
-      </c>
-      <c r="E54" s="10">
+    </row>
+    <row r="54" spans="1:11" ht="39">
+      <c r="A54" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="B54" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C54" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D54" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E54" s="6"/>
+      <c r="F54" s="6"/>
+      <c r="G54" s="6"/>
+      <c r="H54" s="6"/>
+      <c r="I54" s="6"/>
+      <c r="J54" s="6"/>
+    </row>
+    <row r="55" spans="1:11" ht="13">
+      <c r="A55" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="B55" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C55" s="6"/>
+      <c r="D55" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E55" s="6">
+        <v>3037556</v>
+      </c>
+      <c r="F55" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="G55" s="6">
+        <v>8840</v>
+      </c>
+      <c r="H55" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="I55" s="6"/>
+      <c r="J55" s="6"/>
+    </row>
+    <row r="56" spans="1:11" ht="13">
+      <c r="A56" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="B56" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C56" s="6"/>
+      <c r="D56" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E56" s="6">
+        <v>3016723</v>
+      </c>
+      <c r="F56" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="G56" s="6">
+        <v>8840</v>
+      </c>
+      <c r="H56" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="I56" s="6"/>
+      <c r="J56" s="6"/>
+    </row>
+    <row r="57" spans="1:11" ht="13">
+      <c r="A57" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B57" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C57" s="6"/>
+      <c r="D57" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E57" s="9">
+        <v>3027114</v>
+      </c>
+      <c r="F57" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="G57" s="6">
+        <v>8840</v>
+      </c>
+      <c r="H57" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="I57" s="6"/>
+      <c r="J57" s="6"/>
+      <c r="K57" s="6"/>
+    </row>
+    <row r="58" spans="1:11" ht="76" customHeight="1">
+      <c r="A58" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="B58" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="C58" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="D58" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="E58" s="10">
         <v>4003394</v>
       </c>
-      <c r="F54" s="10" t="s">
-        <v>107</v>
-      </c>
-      <c r="G54" s="10"/>
-      <c r="H54" s="10"/>
-      <c r="I54" s="12" t="s">
-        <v>158</v>
-      </c>
-      <c r="J54" s="12" t="s">
-        <v>111</v>
+      <c r="F58" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="G58" s="10"/>
+      <c r="H58" s="10"/>
+      <c r="I58" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="J58" s="12" t="s">
+        <v>102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>